<commit_message>
Tests updates after sort
</commit_message>
<xml_diff>
--- a/test/Bugs.xlsx
+++ b/test/Bugs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="181">
   <si>
     <t>Test cycle</t>
   </si>
@@ -55,21 +55,21 @@
     <t>Bug</t>
   </si>
   <si>
+    <t>Improvement</t>
+  </si>
+  <si>
+    <t>Failed to load resources: https://fonts.googleapis.com/%20%20%2 0css?family=Bowlby+One+SC|Poppins   ,   bootstrap-select.js.map</t>
+  </si>
+  <si>
+    <t>Compress image</t>
+  </si>
+  <si>
     <t>Agent List is empty for posting listing</t>
   </si>
   <si>
-    <t>Failed to load resources: https://fonts.googleapis.com/%20%20%2 0css?family=Bowlby+One+SC|Poppins   ,   bootstrap-select.js.map</t>
-  </si>
-  <si>
     <t>Farzaneh</t>
   </si>
   <si>
-    <t>Improvement</t>
-  </si>
-  <si>
-    <t>Compress image</t>
-  </si>
-  <si>
     <t>Vijay</t>
   </si>
   <si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>Medium</t>
   </si>
   <si>
     <t>high</t>
@@ -112,40 +115,34 @@
     <t>5 mins</t>
   </si>
   <si>
-    <t>Image loads faster</t>
-  </si>
-  <si>
-    <t>Medium</t>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>5m</t>
   </si>
   <si>
     <t>Alignment in search cards</t>
   </si>
   <si>
+    <t>Delete Button in edit listing dose not work</t>
+  </si>
+  <si>
     <t>completed</t>
   </si>
   <si>
     <t>15 mins</t>
   </si>
   <si>
-    <t>5m</t>
-  </si>
-  <si>
-    <t>Fixed</t>
-  </si>
-  <si>
     <t>Login/signup button dose not work FireFox</t>
   </si>
   <si>
     <t>FireFox</t>
   </si>
   <si>
-    <t>Not completed</t>
-  </si>
-  <si>
-    <t>I finsihed it : vijay</t>
-  </si>
-  <si>
-    <t>Delete Button in edit listing dose not work</t>
+    <t>Add City to listing cards</t>
+  </si>
+  <si>
+    <t>Compeleted by Vijay (Was assigned to Saad)</t>
   </si>
   <si>
     <t>Saad</t>
@@ -154,22 +151,7 @@
     <t>Not fixed</t>
   </si>
   <si>
-    <t>User profile is not displaying</t>
-  </si>
-  <si>
-    <t>Please check again</t>
-  </si>
-  <si>
-    <t>Add City to listing cards</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bid is not sent </t>
-  </si>
-  <si>
-    <t>static files path</t>
-  </si>
-  <si>
-    <t>1h</t>
   </si>
   <si>
     <r>
@@ -183,42 +165,57 @@
     </r>
   </si>
   <si>
+    <t>User profile is not displaying</t>
+  </si>
+  <si>
+    <t>Make font files Local</t>
+  </si>
+  <si>
+    <t>Please check again</t>
+  </si>
+  <si>
+    <t>Fixed the Url error</t>
+  </si>
+  <si>
+    <t>Restrict negative values</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Improve Search &amp; filter UI</t>
+  </si>
+  <si>
+    <t>static files path</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
     <t>Critical Bug</t>
   </si>
   <si>
-    <t>Make font files Local</t>
-  </si>
-  <si>
-    <t>Fixed the Url error</t>
-  </si>
-  <si>
-    <t>Restrict negative values</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
     <t>Add user name to page header</t>
   </si>
   <si>
-    <t>Improve Search &amp; filter UI</t>
-  </si>
-  <si>
     <t>Signup button dose not have properCSS</t>
   </si>
   <si>
-    <t>Not Fixed</t>
-  </si>
-  <si>
     <t>Sending status 200 even after entering wrong login credentials</t>
   </si>
   <si>
+    <t>Email Id should not be editable front-end and back-end</t>
+  </si>
+  <si>
     <t>Imam</t>
   </si>
   <si>
     <t>Search button in not working without locaion and city  : https://www.sfsuse.com/fa17g20/undefined</t>
   </si>
   <si>
+    <t>User-type should not be passed to /signup : security problem</t>
+  </si>
+  <si>
     <t xml:space="preserve">All </t>
   </si>
   <si>
@@ -228,64 +225,61 @@
     <t>15min</t>
   </si>
   <si>
+    <t>How do we handle this?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Exchange the location and city fields </t>
   </si>
   <si>
+    <t>Only current user can edit his profile : security problem</t>
+  </si>
+  <si>
     <t>Changed in Customer dashboard:vijay</t>
   </si>
   <si>
-    <t>Email Id should not be editable front-end and back-end</t>
+    <t>Who else should be allowed to edit?</t>
   </si>
   <si>
     <t>bg-footer.jpg not found</t>
   </si>
   <si>
-    <t>User-type should not be passed to /signup : security problem</t>
+    <t>What is the usage of "https://www.sfsuse.com/fa17g20/user/profile"</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
   <si>
     <t>1 min</t>
   </si>
   <si>
-    <t>How do we handle this?</t>
-  </si>
-  <si>
     <t>Password is not encrypted</t>
   </si>
   <si>
-    <t>Only current user can edit his profile : security problem</t>
-  </si>
-  <si>
-    <t>Who else should be allowed to edit?</t>
+    <t>Extracting City names from existing listing dose not make sense</t>
+  </si>
+  <si>
+    <t>Imam and farrukh</t>
+  </si>
+  <si>
+    <t>Related to number:19 --&gt; initial status for listing should be inactive not expired</t>
   </si>
   <si>
     <t xml:space="preserve">After successful login the button of signin is still there </t>
   </si>
   <si>
-    <t>What is the usage of "https://www.sfsuse.com/fa17g20/user/profile"</t>
-  </si>
-  <si>
-    <t>Low</t>
+    <t>backend</t>
   </si>
   <si>
     <t>5min</t>
   </si>
   <si>
-    <t>Extracting City names from existing listing dose not make sense</t>
-  </si>
-  <si>
     <t>Wrong redirection from signup page to home page - click on Home link</t>
   </si>
   <si>
-    <t>Imam and farrukh</t>
-  </si>
-  <si>
     <t>Working well now in local will know after pulling latest code</t>
   </si>
   <si>
-    <t>Related to number:19 --&gt; initial status for listing should be inactive not expired</t>
-  </si>
-  <si>
-    <t>backend</t>
+    <t xml:space="preserve">Remove expiry date from front-end and back-end : there is no need when we have expired as a status </t>
   </si>
   <si>
     <t>5 min</t>
@@ -332,10 +326,13 @@
     <t>Logout dose not work for customer</t>
   </si>
   <si>
+    <t>Compeleted</t>
+  </si>
+  <si>
     <t>Safari</t>
   </si>
   <si>
-    <t xml:space="preserve">Remove expiry date from front-end and back-end : there is no need when we have expired as a status </t>
+    <t>Shall we remove this field totally?, it was one of the reason for our application to crash</t>
   </si>
   <si>
     <t>10min</t>
@@ -359,7 +356,13 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Sort query is wrong </t>
+  </si>
+  <si>
     <t>Listing directly displayed without Agent approval</t>
+  </si>
+  <si>
+    <t>/agent/listing/update , agenId should not be editable, back-end</t>
   </si>
   <si>
     <r>
@@ -381,15 +384,12 @@
     <t>Agent Dashbord tabs change without refreshing the content</t>
   </si>
   <si>
-    <t>Compeleted</t>
-  </si>
-  <si>
-    <t>Shall we remove this field totally?, it was one of the reason for our application to crash</t>
-  </si>
-  <si>
     <t>Need more Description - Farzaneh : By clicking on tab recall ajax to refresh the contect of tab</t>
   </si>
   <si>
+    <t>added only for manage listing</t>
+  </si>
+  <si>
     <t>No nitification after list posting by agents</t>
   </si>
   <si>
@@ -399,10 +399,22 @@
     <t xml:space="preserve">In which tab? </t>
   </si>
   <si>
-    <t xml:space="preserve">Sort query is wrong </t>
-  </si>
-  <si>
-    <t>/agent/listing/update , agenId should not be editable, back-end</t>
+    <t>("Add Profile request received.") for Delete listing</t>
+  </si>
+  <si>
+    <t>Delete listing fails if there is any dependancy to listing : like message</t>
+  </si>
+  <si>
+    <t>listing/image returns 502 if listingId is not found</t>
+  </si>
+  <si>
+    <t>Backend</t>
+  </si>
+  <si>
+    <t>listing/image return 502 if there is no image for a listing</t>
+  </si>
+  <si>
+    <t>update listing should accept images : agent/listing/update</t>
   </si>
   <si>
     <r>
@@ -422,94 +434,52 @@
     </r>
   </si>
   <si>
+    <t>Add listing id to bid message</t>
+  </si>
+  <si>
+    <t>lesss time to implement this feature</t>
+  </si>
+  <si>
     <t>Expiry date is not stored in DB</t>
   </si>
   <si>
+    <t>expiry date format  : better to delete this field</t>
+  </si>
+  <si>
+    <t>Rearrange location and listing fields in cus dashboard</t>
+  </si>
+  <si>
+    <t>Professor</t>
+  </si>
+  <si>
+    <t>10 min</t>
+  </si>
+  <si>
     <t>Data failed message for listing update</t>
   </si>
   <si>
+    <t>Improvemnt</t>
+  </si>
+  <si>
+    <t>add validation for post listing : area -&gt; integer , qoute &gt; price</t>
+  </si>
+  <si>
+    <t>Manage Listing and Post listing have the same UI . (?)</t>
+  </si>
+  <si>
     <t>You have tp give all details as all are mandatory did not put Validations</t>
   </si>
   <si>
+    <t>Add images for edit listing by agents</t>
+  </si>
+  <si>
     <t>City drop down CSS dose not work in home page and listing page</t>
   </si>
   <si>
+    <t>Compelted</t>
+  </si>
+  <si>
     <t>Need more details :  Sometime is rendering like this ---&gt; image</t>
-  </si>
-  <si>
-    <t>Fixing bootstrap select will fix this bug</t>
-  </si>
-  <si>
-    <t>Additional details/ features/photos  are the same for all listings</t>
-  </si>
-  <si>
-    <t>If picture is not uploaded default picture is loaded:vijay</t>
-  </si>
-  <si>
-    <t>Listing details starts with Villa !!</t>
-  </si>
-  <si>
-    <t>("Add Profile request received.") for Delete listing</t>
-  </si>
-  <si>
-    <t>vijay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Backend? </t>
-  </si>
-  <si>
-    <t>Sorts are not working: backend and front end not implemented</t>
-  </si>
-  <si>
-    <t>Delete listing fails if there is any dependancy to listing : like message</t>
-  </si>
-  <si>
-    <t xml:space="preserve">search filter is reset to default after clicking on search button </t>
-  </si>
-  <si>
-    <t>listing/image returns 502 if listingId is not found</t>
-  </si>
-  <si>
-    <t>Backend</t>
-  </si>
-  <si>
-    <t>listing/image return 502 if there is no image for a listing</t>
-  </si>
-  <si>
-    <t>update listing should accept images : agent/listing/update</t>
-  </si>
-  <si>
-    <t>lesss time to implement this feature</t>
-  </si>
-  <si>
-    <t>expiry date format  : better to delete this field</t>
-  </si>
-  <si>
-    <t>Add listing id to bid message</t>
-  </si>
-  <si>
-    <t>10 min</t>
-  </si>
-  <si>
-    <t>Rearrange location and listing fields in cus dashboard</t>
-  </si>
-  <si>
-    <t>Professor</t>
-  </si>
-  <si>
-    <t>Agent dashbord should be sortable for bid price :backend and front end not implemented</t>
-  </si>
-  <si>
-    <t>Manage Listing and Post listing have the same UI . (?)</t>
-  </si>
-  <si>
-    <t>Improvemnt</t>
-  </si>
-  <si>
-    <t>add validation for post listing : area -&gt; integer , qoute &gt; price</t>
-  </si>
-  <si>
-    <t>Add images for edit listing by agents</t>
   </si>
   <si>
     <r>
@@ -523,19 +493,83 @@
     </r>
   </si>
   <si>
+    <t>Removing the Dropdown as its not working most of the time</t>
+  </si>
+  <si>
+    <t>Additional details/ features/photos  are the same for all listings</t>
+  </si>
+  <si>
+    <t>Search button is not working without parameters</t>
+  </si>
+  <si>
+    <t>If picture is not uploaded default picture is loaded:vijay</t>
+  </si>
+  <si>
+    <t>Shows all the results</t>
+  </si>
+  <si>
+    <t>Listing details starts with Villa !!</t>
+  </si>
+  <si>
+    <t>vijay</t>
+  </si>
+  <si>
     <t>Related to bug 30 : Sort calls from Front-end</t>
   </si>
   <si>
-    <t>Search button is not working without parameters</t>
-  </si>
-  <si>
-    <t>Will not be able to do this.</t>
-  </si>
-  <si>
-    <t>vijay &amp; imam</t>
-  </si>
-  <si>
-    <t>Shows all the results</t>
+    <t>Sorts are not working: backend and front end not implemented</t>
+  </si>
+  <si>
+    <t>HOME NEW ACCOUNT / SIGN IN
+ - page header for sign in : remove Home word</t>
+  </si>
+  <si>
+    <t>Expiry date format is not clear : See no 60 --&gt; add validation or date format as placeholder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 min </t>
+  </si>
+  <si>
+    <t xml:space="preserve">City drop down only SOMETIMES shows values  </t>
+  </si>
+  <si>
+    <t>Same reason as 69 bug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search filter is reset to default after clicking on search button </t>
+  </si>
+  <si>
+    <t>Listing title is always "Super Nice Villa", it shoud display listing title</t>
+  </si>
+  <si>
+    <t>Fixed it already last night, Please check again</t>
+  </si>
+  <si>
+    <t>Price, area, bedrooms, biddable display static values</t>
+  </si>
+  <si>
+    <t>Even though there is static value in html it is replaced by js. removed static values now except for status.</t>
+  </si>
+  <si>
+    <t>Features part is static</t>
+  </si>
+  <si>
+    <t>Yes, Had to fill the page</t>
+  </si>
+  <si>
+    <t>Search is not working without parameter, whenever city dropdown list is empty , this problem apprears.</t>
+  </si>
+  <si>
+    <t>It is beacuse of the timing out bug in server i guess latest pull will fix this, will check for this again after pulling</t>
+  </si>
+  <si>
+    <t>Back end is done : bug 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Listings!!! remains at the botton of page after adding a listing by an agent </t>
+  </si>
+  <si>
+    <t>Set minum beds and baths to 0</t>
   </si>
   <si>
     <r>
@@ -549,14 +583,7 @@
     </r>
   </si>
   <si>
-    <t>HOME NEW ACCOUNT / SIGN IN
- - page header for sign in : remove Home word</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activate enter key for search </t>
-  </si>
-  <si>
-    <t>Should keep a listner fo every key press</t>
+    <t>Not Fixed</t>
   </si>
   <si>
     <r>
@@ -570,10 +597,13 @@
     </r>
   </si>
   <si>
-    <t>Expiry date format is not clear : See no 60 --&gt; add validation or date format as placeholder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 min </t>
+    <t>Cant fix</t>
+  </si>
+  <si>
+    <t>Google maps error</t>
+  </si>
+  <si>
+    <t>Agent dashbord should be sortable for bid price :backend and front end not implemented</t>
   </si>
   <si>
     <r>
@@ -587,43 +617,13 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">City drop down only SOMETIMES shows values  </t>
-  </si>
-  <si>
-    <t>Same reason as 69 bug</t>
-  </si>
-  <si>
-    <t>Listing title is always "Super Nice Villa", it shoud display listing title</t>
-  </si>
-  <si>
-    <t>Fixed it already last night, Please check again</t>
-  </si>
-  <si>
-    <t>Price, area, bedrooms, biddable display static values</t>
-  </si>
-  <si>
-    <t>Even though there is static value in html it is replaced by js. removed static values now except for status.</t>
-  </si>
-  <si>
-    <t>Features part is static</t>
-  </si>
-  <si>
-    <t>Yes, Had to fill the page</t>
-  </si>
-  <si>
-    <t>Search is not working without parameter, whenever city dropdown list is empty , this problem apprears.</t>
-  </si>
-  <si>
-    <t>It is beacuse of the timing out bug in server i guess latest pull will fix this, will check for this again after pulling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Listings!!! remains at the botton of page after adding a listing by an agent </t>
-  </si>
-  <si>
-    <t>Set minum beds and baths to 0</t>
-  </si>
-  <si>
     <t xml:space="preserve">it will allow to type -1 but it will not go down below 0 when using arrows, cant do more without framework. </t>
+  </si>
+  <si>
+    <t>Will not be able to do this.</t>
+  </si>
+  <si>
+    <t>vijay &amp; imam</t>
   </si>
   <si>
     <t>After editing listing , list of listings shows one item many times. whatsapp image</t>
@@ -640,7 +640,13 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">activate enter key for search </t>
+  </si>
+  <si>
     <t>clicking on manage listing should refresh the list</t>
+  </si>
+  <si>
+    <t>Should keep a listner fo every key press</t>
   </si>
   <si>
     <t>Need time for this feature</t>
@@ -682,7 +688,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -701,11 +707,15 @@
       <color rgb="FF999999"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <color rgb="FF505050"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <i/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF505050"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -751,14 +761,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFE599"/>
-        <bgColor rgb="FFFFE599"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -793,7 +803,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -801,10 +811,10 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -822,36 +832,45 @@
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="7" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="8" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="8" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="7" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="6" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="2" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="6" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="6" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -965,20 +984,20 @@
         <v>11</v>
       </c>
       <c r="M1" s="2"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="5">
@@ -988,10 +1007,10 @@
         <v>1.0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>18</v>
@@ -1008,10 +1027,10 @@
         <v>18</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="5" t="s">
         <v>27</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="M2" s="6"/>
     </row>
@@ -1026,7 +1045,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>18</v>
@@ -1036,16 +1055,18 @@
         <v>19</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="6"/>
+        <v>33</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="M3" s="6"/>
     </row>
     <row r="4">
@@ -1062,26 +1083,26 @@
         <v>34</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>35</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>37</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M4" s="6"/>
     </row>
@@ -1093,30 +1114,30 @@
         <v>4.0</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="M5" s="6"/>
     </row>
@@ -1128,28 +1149,28 @@
         <v>5.0</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="M6" s="6"/>
     </row>
@@ -1164,29 +1185,29 @@
         <v>12</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="G7" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="L7" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="M7" s="6"/>
     </row>
@@ -1198,16 +1219,16 @@
         <v>7.0</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>63</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>19</v>
@@ -1216,10 +1237,10 @@
         <v>20</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
@@ -1236,29 +1257,29 @@
         <v>12</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="M9" s="6"/>
     </row>
@@ -1273,27 +1294,27 @@
         <v>12</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="M10" s="6"/>
     </row>
@@ -1308,27 +1329,27 @@
         <v>12</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="M11" s="6"/>
     </row>
@@ -1346,26 +1367,26 @@
         <v>78</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="M12" s="6"/>
     </row>
@@ -1380,26 +1401,26 @@
         <v>12</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
@@ -1415,14 +1436,14 @@
         <v>12</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>20</v>
@@ -1432,10 +1453,10 @@
         <v>18</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="M14" s="6"/>
     </row>
@@ -1450,20 +1471,20 @@
         <v>12</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>18</v>
@@ -1483,10 +1504,10 @@
         <v>12</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="5" t="s">
@@ -1496,14 +1517,14 @@
         <v>20</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="K16" s="6"/>
       <c r="L16" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="M16" s="6"/>
     </row>
@@ -1518,27 +1539,27 @@
         <v>12</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K17" s="6"/>
       <c r="L17" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="M17" s="6"/>
     </row>
@@ -1553,29 +1574,29 @@
         <v>12</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="G18" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="M18" s="6"/>
     </row>
@@ -1590,21 +1611,21 @@
         <v>12</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -1624,22 +1645,22 @@
         <v>99</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="M20" s="6"/>
     </row>
@@ -1654,21 +1675,21 @@
         <v>12</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -1685,23 +1706,27 @@
         <v>12</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H22" s="17"/>
+        <v>47</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I22" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
+      <c r="M22" s="5" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="5">
@@ -1717,11 +1742,11 @@
         <v>105</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>20</v>
@@ -1732,7 +1757,7 @@
       </c>
       <c r="K23" s="6"/>
       <c r="L23" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="M23" s="6"/>
     </row>
@@ -1750,14 +1775,14 @@
         <v>106</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H24" s="6"/>
-      <c r="I24" s="19" t="s">
+      <c r="I24" s="18" t="s">
         <v>107</v>
       </c>
       <c r="J24" s="5" t="s">
@@ -1778,21 +1803,21 @@
         <v>12</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
@@ -1809,21 +1834,21 @@
         <v>12</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I26" s="6"/>
       <c r="J26" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
@@ -1840,17 +1865,17 @@
         <v>12</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="5" t="s">
@@ -1858,10 +1883,10 @@
       </c>
       <c r="K27" s="6"/>
       <c r="L27" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28">
@@ -1875,26 +1900,28 @@
         <v>12</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H28" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="I28" s="5" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
       <c r="L28" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29">
@@ -1908,20 +1935,20 @@
         <v>12</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>18</v>
@@ -1941,60 +1968,58 @@
         <v>12</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I30" s="5"/>
       <c r="J30" s="5" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="K30" s="6"/>
       <c r="L30" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="M30" s="6"/>
     </row>
     <row r="31">
-      <c r="A31" s="5">
+      <c r="A31" s="20">
         <v>1.0</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="20">
         <v>30.0</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="6"/>
-      <c r="G31" s="5" t="s">
-        <v>52</v>
+      <c r="C31" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="22"/>
+      <c r="G31" s="20" t="s">
+        <v>47</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I31" s="6"/>
       <c r="J31" s="5" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="K31" s="6"/>
-      <c r="L31" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="M31" s="6"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="5"/>
     </row>
     <row r="32">
       <c r="A32" s="5">
@@ -2007,16 +2032,16 @@
         <v>12</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H32" s="21"/>
+        <v>21</v>
+      </c>
+      <c r="H32" s="23"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
@@ -2024,49 +2049,49 @@
       <c r="M32" s="6"/>
     </row>
     <row r="33">
-      <c r="A33" s="22">
+      <c r="A33" s="24">
         <v>1.0</v>
       </c>
-      <c r="B33" s="22">
+      <c r="B33" s="24">
         <v>32.0</v>
       </c>
-      <c r="C33" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="F33" s="23"/>
-      <c r="G33" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="H33" s="23"/>
-      <c r="I33" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="J33" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="K33" s="23"/>
-      <c r="L33" s="23"/>
-      <c r="M33" s="23"/>
-      <c r="N33" s="24"/>
-      <c r="O33" s="24"/>
-      <c r="P33" s="24"/>
-      <c r="Q33" s="24"/>
-      <c r="R33" s="24"/>
-      <c r="S33" s="24"/>
-      <c r="T33" s="24"/>
-      <c r="U33" s="24"/>
-      <c r="V33" s="24"/>
-      <c r="W33" s="24"/>
-      <c r="X33" s="24"/>
-      <c r="Y33" s="24"/>
-      <c r="Z33" s="24"/>
-      <c r="AA33" s="24"/>
+      <c r="C33" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="E33" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="26"/>
+      <c r="G33" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="H33" s="26"/>
+      <c r="I33" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="J33" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
+      <c r="M33" s="26"/>
+      <c r="N33" s="28"/>
+      <c r="O33" s="28"/>
+      <c r="P33" s="28"/>
+      <c r="Q33" s="28"/>
+      <c r="R33" s="28"/>
+      <c r="S33" s="28"/>
+      <c r="T33" s="28"/>
+      <c r="U33" s="28"/>
+      <c r="V33" s="28"/>
+      <c r="W33" s="28"/>
+      <c r="X33" s="28"/>
+      <c r="Y33" s="28"/>
+      <c r="Z33" s="28"/>
+      <c r="AA33" s="28"/>
     </row>
     <row r="34">
       <c r="A34" s="5">
@@ -2076,24 +2101,24 @@
         <v>33.0</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="5" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
@@ -2153,20 +2178,20 @@
         <v>11</v>
       </c>
       <c r="M1" s="2"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="5">
@@ -2179,21 +2204,21 @@
         <v>12</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
@@ -2210,27 +2235,27 @@
         <v>12</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="M3" s="5"/>
     </row>
@@ -2245,17 +2270,17 @@
         <v>12</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="5" t="s">
@@ -2263,7 +2288,7 @@
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="M4" s="6"/>
     </row>
@@ -2275,20 +2300,20 @@
         <v>37.0</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="5" t="s">
@@ -2296,7 +2321,7 @@
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="M5" s="6"/>
     </row>
@@ -2311,27 +2336,27 @@
         <v>12</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="M6" s="6"/>
     </row>
@@ -2343,23 +2368,23 @@
         <v>39.0</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>18</v>
@@ -2376,17 +2401,17 @@
         <v>40.0</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>20</v>
@@ -2407,17 +2432,17 @@
         <v>41.0</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>20</v>
@@ -2443,6 +2468,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="4" max="4" width="72.14"/>
+    <col customWidth="1" min="9" max="9" width="32.0"/>
     <col customWidth="1" min="12" max="12" width="34.29"/>
     <col customWidth="1" min="13" max="13" width="37.29"/>
   </cols>
@@ -2481,24 +2507,24 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="5">
@@ -2514,15 +2540,17 @@
         <v>14</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="J2" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K2" s="6"/>
       <c r="L2" s="8"/>
     </row>
@@ -2537,23 +2565,25 @@
         <v>12</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" s="6"/>
+        <v>44</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K3" s="6"/>
       <c r="L3" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
@@ -2564,17 +2594,17 @@
         <v>44.0</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -2593,25 +2623,27 @@
         <v>12</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>35</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
+      <c r="J5" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K5" s="6"/>
-      <c r="L5" s="12" t="s">
-        <v>56</v>
+      <c r="L5" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6">
@@ -2625,23 +2657,25 @@
         <v>12</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
+      <c r="J6" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K6" s="6"/>
       <c r="L6" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -2655,18 +2689,18 @@
         <v>12</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
@@ -2683,18 +2717,18 @@
         <v>12</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
@@ -2708,17 +2742,17 @@
         <v>49.0</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2737,18 +2771,18 @@
         <v>12</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -2765,73 +2799,73 @@
         <v>12</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="8"/>
     </row>
     <row r="12">
-      <c r="A12" s="14">
+      <c r="A12" s="12">
         <v>3.0</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="12">
         <v>52.0</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="15" t="s">
+      <c r="C12" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="E12" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="16"/>
-      <c r="G12" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>97</v>
-      </c>
       <c r="L12" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="18"/>
-      <c r="Z12" s="18"/>
-      <c r="AA12" s="18"/>
+        <v>28</v>
+      </c>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="16"/>
+      <c r="Z12" s="16"/>
+      <c r="AA12" s="16"/>
     </row>
     <row r="13">
       <c r="A13" s="5">
@@ -2844,19 +2878,19 @@
         <v>12</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="8"/>
@@ -2871,15 +2905,15 @@
       <c r="C14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="20" t="s">
-        <v>109</v>
+      <c r="D14" s="17" t="s">
+        <v>100</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
@@ -2895,23 +2929,25 @@
         <v>55.0</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="J15" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="K15" s="6"/>
       <c r="L15" s="8"/>
     </row>
@@ -2926,18 +2962,20 @@
         <v>12</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H16" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="I16" s="5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
@@ -2954,10 +2992,10 @@
         <v>12</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="5" t="s">
@@ -2965,7 +3003,7 @@
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="5" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
@@ -2982,18 +3020,18 @@
         <v>12</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
@@ -3010,18 +3048,18 @@
         <v>12</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="5" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -3035,30 +3073,30 @@
         <v>60.0</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>131</v>
+        <v>13</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>118</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="I20" s="6"/>
+      <c r="J20" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="L20" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="I20" s="6"/>
-      <c r="J20" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="L20" s="10" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="21">
@@ -3072,25 +3110,27 @@
         <v>12</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="J21" s="6"/>
+        <v>131</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K21" s="6"/>
       <c r="L21" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22">
@@ -3104,20 +3144,22 @@
         <v>12</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H22" s="6"/>
       <c r="I22" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="J22" s="6"/>
+        <v>136</v>
+      </c>
+      <c r="J22" s="21" t="s">
+        <v>18</v>
+      </c>
       <c r="K22" s="6"/>
       <c r="L22" s="8"/>
     </row>
@@ -3132,23 +3174,25 @@
         <v>12</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
+      <c r="J23" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K23" s="6"/>
       <c r="L23" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24">
@@ -3157,10 +3201,10 @@
         <v>64.0</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>152</v>
+        <v>13</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>142</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="6"/>
@@ -3169,14 +3213,14 @@
         <v>20</v>
       </c>
       <c r="I24" s="5"/>
-      <c r="J24" s="14" t="s">
-        <v>15</v>
+      <c r="J24" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25">
@@ -3190,25 +3234,27 @@
         <v>12</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="J25" s="6"/>
+        <v>145</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K25" s="6"/>
-      <c r="L25" s="12" t="s">
-        <v>56</v>
+      <c r="L25" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="26">
@@ -3222,25 +3268,27 @@
         <v>12</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="J26" s="6"/>
+        <v>148</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K26" s="6"/>
       <c r="L26" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27">
@@ -3254,25 +3302,27 @@
         <v>12</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="J27" s="6"/>
+        <v>150</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K27" s="6"/>
       <c r="L27" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28">
@@ -3286,22 +3336,24 @@
         <v>12</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="J28" s="6"/>
+        <v>152</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K28" s="6"/>
       <c r="L28" s="8"/>
     </row>
@@ -3316,25 +3368,27 @@
         <v>12</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="J29" s="6"/>
+        <v>154</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K29" s="6"/>
       <c r="L29" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30">
@@ -3348,23 +3402,25 @@
         <v>12</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
+      <c r="J30" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K30" s="6"/>
       <c r="L30" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31">
@@ -3378,26 +3434,28 @@
         <v>12</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H31" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
+      <c r="J31" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K31" s="6"/>
-      <c r="L31" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="M31" s="25" t="s">
-        <v>167</v>
+      <c r="L31" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="M31" s="27" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="32">
@@ -3414,17 +3472,21 @@
         <v>168</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H32" s="21"/>
+        <v>47</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I32" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="J32" s="6"/>
+      <c r="J32" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K32" s="6"/>
       <c r="L32" s="8"/>
     </row>
@@ -3439,20 +3501,24 @@
         <v>12</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H33" s="21"/>
+        <v>47</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I33" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="J33" s="6"/>
+        <v>173</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K33" s="6"/>
       <c r="L33" s="8"/>
     </row>
@@ -3467,22 +3533,24 @@
         <v>12</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>30</v>
+        <v>47</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="J34" s="6"/>
+        <v>175</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K34" s="6"/>
       <c r="L34" s="8"/>
     </row>
@@ -3494,17 +3562,17 @@
         <v>75.0</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F35" s="6"/>
       <c r="G35" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -3523,24 +3591,24 @@
         <v>12</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F36" s="6"/>
       <c r="G36" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I36" s="6"/>
       <c r="J36" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="L36" s="8"/>
     </row>
@@ -3555,14 +3623,14 @@
         <v>12</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -3578,28 +3646,28 @@
         <v>78.0</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H38" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I38" s="6"/>
       <c r="J38" s="5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="K38" s="6"/>
       <c r="L38" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -3614,7 +3682,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="65.14"/>
+    <col customWidth="1" min="4" max="4" width="102.0"/>
     <col customWidth="1" min="12" max="12" width="29.0"/>
   </cols>
   <sheetData>
@@ -3656,20 +3724,20 @@
         <v>11</v>
       </c>
       <c r="M1" s="2"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="5">
@@ -3679,29 +3747,31 @@
         <v>79.0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L2" s="6"/>
+        <v>61</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="M2" s="6"/>
     </row>
     <row r="3">
@@ -3712,17 +3782,17 @@
         <v>80.0</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>20</v>
@@ -3732,9 +3802,11 @@
         <v>18</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="L3" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="M3" s="6"/>
     </row>
     <row r="4">
@@ -3745,17 +3817,17 @@
         <v>81.0</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -3774,17 +3846,17 @@
         <v>82.0</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -3799,24 +3871,26 @@
       <c r="A6" s="5">
         <v>4.0</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="19">
         <v>83.0</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="5" t="s">
-        <v>52</v>
+      <c r="C6" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="23"/>
+      <c r="G6" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="I6" s="5" t="s">
+        <v>155</v>
+      </c>
       <c r="J6" s="5" t="s">
         <v>18</v>
       </c>
@@ -3835,22 +3909,26 @@
         <v>12</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I7" s="6"/>
       <c r="J7" s="5" t="s">
         <v>18</v>
       </c>
       <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
+      <c r="L7" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="M7" s="6"/>
     </row>
     <row r="8">
@@ -3864,18 +3942,24 @@
         <v>12</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
@@ -3891,20 +3975,26 @@
         <v>12</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
+      <c r="J9" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
+      <c r="L9" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="M9" s="6"/>
     </row>
     <row r="10">

</xml_diff>